<commit_message>
EPBDS-6913 Add more test cases for empty and null values
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Boolean.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Boolean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="primitive" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="41">
-  <si>
-    <t>Result</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="42">
   <si>
     <t>Array</t>
   </si>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>yes, ,yes</t>
+  </si>
+  <si>
+    <t>, ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -537,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -563,41 +566,41 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -606,308 +609,323 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -922,10 +940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +957,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -948,41 +966,41 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -991,391 +1009,425 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
-        <v>37</v>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>38</v>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1384,5 +1436,6 @@
     <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>